<commit_message>
modified so many pages and added some features
</commit_message>
<xml_diff>
--- a/author_files/les étudiants.xlsx
+++ b/author_files/les étudiants.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delli7\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delli7\Desktop\cours_feedback\author_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6232C6C-49DA-4781-8E3D-EF10720C8859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15584F5-0335-4EDE-B877-4442508D704D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2C6028CB-D5F1-4ED9-8738-F3DBB0E54585}"/>
   </bookViews>
@@ -1357,7 +1357,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1675,7 +1675,7 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1685,7 +1685,7 @@
     <col min="3" max="3" width="21.54296875" customWidth="1"/>
     <col min="4" max="4" width="14.90625" customWidth="1"/>
     <col min="5" max="5" width="10.90625" style="1"/>
-    <col min="6" max="6" width="14.08984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
@@ -2917,8 +2917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2C2980-1FF4-4EE3-AFF2-B50A93BB5ADE}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>